<commit_message>
Update Annex III complete. Update TaxPaid.
</commit_message>
<xml_diff>
--- a/core/templates/static/CC - guide.xlsx
+++ b/core/templates/static/CC - guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TiiTii\Desktop\Q_Wrkr\core\templates\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A397BB66-EE95-4167-BA16-F9E25E780AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FBE039-0163-4A74-B2E4-EBBD67006C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="6936" xr2:uid="{B133F4AA-A48A-4334-AAD3-56F9208FC82D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B133F4AA-A48A-4334-AAD3-56F9208FC82D}"/>
   </bookViews>
   <sheets>
     <sheet name="AnnexIII-Local Pur" sheetId="2" r:id="rId1"/>
@@ -50,6 +50,7 @@
     <definedName name="__SR1">#REF!</definedName>
     <definedName name="__SR2">#REF!</definedName>
     <definedName name="__wb2" hidden="1">{#N/A,#N/A,FALSE,"1998_SK_DB2";#N/A,#N/A,FALSE,"1999_SK_DB2";#N/A,#N/A,FALSE,"2000_SK_DB2";#N/A,#N/A,FALSE,"SK_VE";#N/A,#N/A,FALSE,"1998_CZ_DB2";#N/A,#N/A,FALSE,"1999_CZ_DB2";#N/A,#N/A,FALSE,"2000_CZ_DB2";#N/A,#N/A,FALSE,"CZ_VE";#N/A,#N/A,FALSE,"1998_XX_DB2";#N/A,#N/A,FALSE,"1999_XX_DB2";#N/A,#N/A,FALSE,"2000_XX_DB2";#N/A,#N/A,FALSE,"XX_VE";#N/A,#N/A,FALSE,"SoKo";#N/A,#N/A,FALSE,"SoErg";#N/A,#N/A,FALSE,"Kon"}</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AnnexIII-Local Pur'!$A$1:$AT$1</definedName>
     <definedName name="_Order1" hidden="1">255</definedName>
     <definedName name="_Order2" hidden="1">255</definedName>
     <definedName name="_PR1">[2]Sheet!#REF!</definedName>
@@ -129,7 +130,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>ល.រ</t>
   </si>
@@ -259,7 +260,10 @@
     <t>SUPPLIER</t>
   </si>
   <si>
-    <t>សម្កាល់</t>
+    <t>មតិអ្នកប្រើប្រាស់</t>
+  </si>
+  <si>
+    <t>សម្គាល់</t>
   </si>
 </sst>
 </file>
@@ -358,7 +362,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC59EE2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -516,7 +526,7 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -528,9 +538,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -544,19 +551,25 @@
     <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2782,21 +2795,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C46CD0C5-11A5-4426-9DB9-BD312A5ECF25}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AS3"/>
+  <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="25.77734375" customWidth="1"/>
-    <col min="7" max="8" width="25.77734375" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="25.77734375" style="10" customWidth="1"/>
-    <col min="10" max="44" width="25.77734375" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="11"/>
+    <col min="5" max="5" width="18.77734375" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="11"/>
+    <col min="7" max="8" width="0" style="11" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.77734375" style="14"/>
+    <col min="10" max="20" width="18.77734375" style="11"/>
+    <col min="21" max="21" width="30.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="18.77734375" style="11"/>
+    <col min="25" max="25" width="22" style="11" customWidth="1"/>
+    <col min="26" max="26" width="21.44140625" style="11" customWidth="1"/>
+    <col min="27" max="16384" width="18.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="6" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="5" customFormat="1" ht="22.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2821,209 +2845,215 @@
       <c r="H1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="V1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AM1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AS1" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="11"/>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="10"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="4"/>
-      <c r="AQ3" s="4"/>
-      <c r="AR3" s="4"/>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12"/>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12"/>
+      <c r="AO3" s="12"/>
+      <c r="AP3" s="12"/>
+      <c r="AQ3" s="12"/>
+      <c r="AR3" s="12"/>
+      <c r="AS3" s="12"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AT1" xr:uid="{C46CD0C5-11A5-4426-9DB9-BD312A5ECF25}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>